<commit_message>
Fay kodları dışındaki kısımlar tamamlandı Ayarlar adımı eklendi
</commit_message>
<xml_diff>
--- a/FuzzyMsc/App_Data/Tmp/FileUploads/burdur-jeoteknik-kesit-verileri.xlsx
+++ b/FuzzyMsc/App_Data/Tmp/FileUploads/burdur-jeoteknik-kesit-verileri.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erkanyuksel/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13725"/>
   </bookViews>
   <sheets>
     <sheet name="REZİSTİVİTE" sheetId="1" r:id="rId1"/>
@@ -17,14 +12,6 @@
     <sheet name="SONDAJ" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -208,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,6 +241,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -548,21 +538,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="10.5" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -609,7 +599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -635,7 +625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -667,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -699,7 +689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -737,7 +727,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -772,7 +762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -816,7 +806,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -830,28 +820,31 @@
         <v>1.6</v>
       </c>
       <c r="F8">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G8">
         <v>9.4</v>
       </c>
       <c r="H8">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="I8">
         <v>13.6</v>
       </c>
       <c r="J8">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="K8">
         <v>19.600000000000001</v>
       </c>
-      <c r="M8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>144</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>1</v>
       </c>
@@ -859,12 +852,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
@@ -872,7 +865,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>48</v>
       </c>
@@ -880,7 +873,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>50</v>
       </c>
@@ -888,7 +881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>52</v>
       </c>
@@ -899,7 +892,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>55</v>
       </c>
@@ -914,16 +907,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -961,7 +954,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -996,7 +989,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1031,7 +1024,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1066,7 +1059,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1101,7 +1094,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1136,7 +1129,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1165,12 +1158,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>57</v>
       </c>
@@ -1189,9 +1182,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1226,7 +1219,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1255,7 +1248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1290,7 +1283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>